<commit_message>
3.1.20: Adapt primitive, primitive array, optonal body payload.
</commit_message>
<xml_diff>
--- a/meta/plainApi/BlancoApiPlainArraySample.xlsx
+++ b/meta/plainApi/BlancoApiPlainArraySample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/plainApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5095EE66-4ABE-FE4C-A53A-CBE77EC61A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C57D4E-B09F-C946-97AA-8C67618DC940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="4400" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="860" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -20,11 +20,13 @@
     <sheet name="post_input" sheetId="37" r:id="rId5"/>
     <sheet name="post_output" sheetId="38" r:id="rId6"/>
     <sheet name="post_error" sheetId="39" r:id="rId7"/>
-    <sheet name="readme" sheetId="17" r:id="rId8"/>
-    <sheet name="config" sheetId="3" r:id="rId9"/>
+    <sheet name="put_input" sheetId="40" r:id="rId8"/>
+    <sheet name="put_output" sheetId="41" r:id="rId9"/>
+    <sheet name="readme" sheetId="17" r:id="rId10"/>
+    <sheet name="config" sheetId="3" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="isImport">config!$E$5:$E$6</definedName>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="252">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2554,6 +2556,29 @@
     </rPh>
     <rPh sb="12" eb="14">
       <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>電文がOption</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>/* ペイロード電文が省略可能 */</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">ショウリャク </t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">カノウ </t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -5440,6 +5465,490 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="35" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19">
+      <c r="A1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1"/>
+      <c r="C16" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="C30" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="C31" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="C33" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="C34" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="C36" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="C38" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="C40" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="C41" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="C42" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="C43" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="C45" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="C46" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="C48" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="C49" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="B50" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="C51" s="35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="C52" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="C56" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="C57" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="24" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="E1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="124" t="s">
+        <v>201</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="125" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="126"/>
+      <c r="H7" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="C8" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D&amp;  &amp;T</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -6916,7 +7425,7 @@
   </sheetPr>
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -9220,8 +9729,8 @@
   </sheetPr>
   <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10729,7 +11238,7 @@
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13022,485 +13531,2697 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A27E73-5CBF-4F4F-8103-4557B07887B0}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="4.5" style="35" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="35"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
+    <col min="8" max="14" width="22.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.83203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="43.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.1640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="6.1640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="18.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.33203125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.83203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="8.83203125" style="1"/>
+    <col min="33" max="33" width="9.1640625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19">
+    <row r="1" spans="1:19" ht="19">
       <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:19">
       <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1"/>
-      <c r="C16" s="35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="C18" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="C29" s="35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="C30" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="C31" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="C32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="C33" s="35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="C34" s="35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="C36" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="C38" s="35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="C40" s="35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="C41" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="C42" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="C43" s="35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="C45" s="35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="C46" s="35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="C48" s="35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="C49" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="B50" s="35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="C51" s="35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="C52" s="35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="C56" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="C57" s="35" t="s">
-        <v>88</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="117" t="str">
+        <f>process!D6&amp;PROPER(C9)&amp;IF(C8="要求電文(C→S)", "Request", "Response")</f>
+        <v>BlancoApiPlainArraySamplePutRequest</v>
+      </c>
+      <c r="D6" s="118"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="110" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="114"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="110" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="115"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="111"/>
+      <c r="C17" s="151" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="151"/>
+      <c r="E17" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="111" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="111"/>
+      <c r="C18" s="151" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="151"/>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="111" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="111"/>
+      <c r="C19" s="150" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="151"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="113"/>
+      <c r="C20" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="112" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="113"/>
+      <c r="C21" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="113"/>
+      <c r="C22" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" t="s">
+        <v>248</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="112" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" s="113"/>
+      <c r="C23" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>251</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="A25" s="146" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="146"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="146"/>
+      <c r="E25" s="146"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="140" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="141"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="95"/>
+      <c r="M26" s="95"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="95"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="95"/>
+      <c r="S26" s="95"/>
+      <c r="U26" s="101"/>
+      <c r="V26" s="101"/>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="A27" s="106"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="102"/>
+      <c r="O27" s="102"/>
+      <c r="P27" s="102"/>
+      <c r="Q27" s="102"/>
+      <c r="R27" s="102"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28" s="107"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="158"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="102"/>
+      <c r="I28" s="102"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102"/>
+      <c r="N28" s="102"/>
+      <c r="O28" s="102"/>
+      <c r="P28" s="102"/>
+      <c r="Q28" s="102"/>
+      <c r="R28" s="102"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="A29" s="108"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="102"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="102"/>
+      <c r="R29" s="102"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" s="143" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="164" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="164"/>
+      <c r="D32" s="164"/>
+      <c r="E32" s="164"/>
+      <c r="F32" s="164"/>
+      <c r="G32" s="164"/>
+      <c r="H32" s="95"/>
+      <c r="I32" s="95"/>
+      <c r="J32" s="95"/>
+      <c r="K32" s="95"/>
+      <c r="L32" s="95"/>
+      <c r="M32" s="95"/>
+      <c r="N32" s="95"/>
+      <c r="O32" s="95"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="95"/>
+      <c r="U32" s="101"/>
+      <c r="V32" s="101"/>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33" s="106">
+        <v>1</v>
+      </c>
+      <c r="B33" s="165" t="s">
+        <v>178</v>
+      </c>
+      <c r="C33" s="165"/>
+      <c r="D33" s="165"/>
+      <c r="E33" s="165"/>
+      <c r="F33" s="165"/>
+      <c r="G33" s="165"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="102"/>
+      <c r="K33" s="102"/>
+      <c r="L33" s="102"/>
+      <c r="M33" s="102"/>
+      <c r="N33" s="102"/>
+      <c r="O33" s="102"/>
+      <c r="P33" s="102"/>
+      <c r="Q33" s="102"/>
+      <c r="R33" s="102"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="A34" s="107"/>
+      <c r="B34" s="166"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="166"/>
+      <c r="E34" s="166"/>
+      <c r="F34" s="166"/>
+      <c r="G34" s="166"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="102"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="102"/>
+      <c r="O34" s="102"/>
+      <c r="P34" s="102"/>
+      <c r="Q34" s="102"/>
+      <c r="R34" s="102"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" s="108"/>
+      <c r="B35" s="167"/>
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="102"/>
+      <c r="I35" s="102"/>
+      <c r="J35" s="102"/>
+      <c r="K35" s="102"/>
+      <c r="L35" s="102"/>
+      <c r="M35" s="102"/>
+      <c r="N35" s="102"/>
+      <c r="O35" s="102"/>
+      <c r="P35" s="102"/>
+      <c r="Q35" s="102"/>
+      <c r="R35" s="102"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37" s="143" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="144"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="145"/>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="164" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="164"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
+      <c r="F38" s="164"/>
+      <c r="G38" s="164"/>
+      <c r="H38" s="95"/>
+      <c r="I38" s="95"/>
+      <c r="J38" s="95"/>
+      <c r="K38" s="95"/>
+      <c r="L38" s="95"/>
+      <c r="M38" s="95"/>
+      <c r="N38" s="95"/>
+      <c r="O38" s="95"/>
+      <c r="P38" s="95"/>
+      <c r="Q38" s="95"/>
+      <c r="R38" s="95"/>
+      <c r="S38" s="95"/>
+      <c r="U38" s="101"/>
+      <c r="V38" s="101"/>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="A39" s="106"/>
+      <c r="B39" s="157"/>
+      <c r="C39" s="157"/>
+      <c r="D39" s="157"/>
+      <c r="E39" s="157"/>
+      <c r="F39" s="157"/>
+      <c r="G39" s="168"/>
+      <c r="H39" s="102"/>
+      <c r="I39" s="102"/>
+      <c r="J39" s="102"/>
+      <c r="K39" s="102"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="102"/>
+      <c r="N39" s="102"/>
+      <c r="O39" s="102"/>
+      <c r="P39" s="102"/>
+      <c r="Q39" s="102"/>
+      <c r="R39" s="102"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" s="107"/>
+      <c r="B40" s="158"/>
+      <c r="C40" s="158"/>
+      <c r="D40" s="158"/>
+      <c r="E40" s="158"/>
+      <c r="F40" s="158"/>
+      <c r="G40" s="169"/>
+      <c r="H40" s="102"/>
+      <c r="I40" s="102"/>
+      <c r="J40" s="102"/>
+      <c r="K40" s="102"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="102"/>
+      <c r="N40" s="102"/>
+      <c r="O40" s="102"/>
+      <c r="P40" s="102"/>
+      <c r="Q40" s="102"/>
+      <c r="R40" s="102"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" s="108"/>
+      <c r="B41" s="159"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="159"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="170"/>
+      <c r="H41" s="102"/>
+      <c r="I41" s="102"/>
+      <c r="J41" s="102"/>
+      <c r="K41" s="102"/>
+      <c r="L41" s="102"/>
+      <c r="M41" s="102"/>
+      <c r="N41" s="102"/>
+      <c r="O41" s="102"/>
+      <c r="P41" s="102"/>
+      <c r="Q41" s="102"/>
+      <c r="R41" s="102"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" s="6"/>
+      <c r="N43" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="109"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="5"/>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" s="176" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="176" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="178" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="176" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="181" t="s">
+        <v>156</v>
+      </c>
+      <c r="F45" s="181" t="s">
+        <v>170</v>
+      </c>
+      <c r="G45" s="176" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="176" t="s">
+        <v>113</v>
+      </c>
+      <c r="I45" s="176" t="s">
+        <v>235</v>
+      </c>
+      <c r="J45" s="181" t="s">
+        <v>236</v>
+      </c>
+      <c r="K45" s="181" t="s">
+        <v>207</v>
+      </c>
+      <c r="L45" s="184" t="s">
+        <v>224</v>
+      </c>
+      <c r="M45" s="176" t="s">
+        <v>224</v>
+      </c>
+      <c r="N45" s="176" t="s">
+        <v>221</v>
+      </c>
+      <c r="O45" s="176" t="s">
+        <v>189</v>
+      </c>
+      <c r="P45" s="179" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q45" s="180"/>
+      <c r="R45" s="179" t="s">
+        <v>16</v>
+      </c>
+      <c r="S45" s="180"/>
+      <c r="T45" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="U45" s="176" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" s="177"/>
+      <c r="B46" s="177"/>
+      <c r="C46" s="177"/>
+      <c r="D46" s="177"/>
+      <c r="E46" s="182"/>
+      <c r="F46" s="182"/>
+      <c r="G46" s="177"/>
+      <c r="H46" s="177"/>
+      <c r="I46" s="177"/>
+      <c r="J46" s="182"/>
+      <c r="K46" s="182"/>
+      <c r="L46" s="183"/>
+      <c r="M46" s="177"/>
+      <c r="N46" s="177"/>
+      <c r="O46" s="183"/>
+      <c r="P46" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q46" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="R46" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="S46" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="T46" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="U46" s="177"/>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" s="7">
+        <v>1</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="23"/>
+      <c r="F47" s="128"/>
+      <c r="G47" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="M47" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="N47" s="120" t="s">
+        <v>197</v>
+      </c>
+      <c r="O47" s="23"/>
+      <c r="P47" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="28">
+        <v>10</v>
+      </c>
+      <c r="R47" s="23"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="28"/>
+      <c r="U47" s="9"/>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48" s="10">
+        <f t="shared" ref="A48:A53" si="0">A47+1</f>
+        <v>2</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="120" t="s">
+        <v>197</v>
+      </c>
+      <c r="O48" s="24"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="29"/>
+      <c r="R48" s="20">
+        <v>0</v>
+      </c>
+      <c r="S48" s="29">
+        <v>100</v>
+      </c>
+      <c r="T48" s="29"/>
+      <c r="U48" s="12"/>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="25"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="120" t="s">
+        <v>200</v>
+      </c>
+      <c r="O49" s="24"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="29"/>
+      <c r="T49" s="29"/>
+      <c r="U49" s="14"/>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="F50" s="73"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="73"/>
+      <c r="I50" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="J50" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="K50" s="73"/>
+      <c r="L50" s="73"/>
+      <c r="M50" s="73"/>
+      <c r="N50" s="120" t="s">
+        <v>200</v>
+      </c>
+      <c r="O50" s="24"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="20"/>
+      <c r="S50" s="29"/>
+      <c r="T50" s="29"/>
+      <c r="U50" s="14"/>
+    </row>
+    <row r="51" spans="1:21">
+      <c r="A51" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51" s="25"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="120"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="30"/>
+      <c r="T51" s="30"/>
+      <c r="U51" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="120"/>
+      <c r="O52" s="24"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="29"/>
+      <c r="R52" s="20"/>
+      <c r="S52" s="29"/>
+      <c r="T52" s="29"/>
+      <c r="U52" s="14"/>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="120"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="29"/>
+      <c r="R53" s="20"/>
+      <c r="S53" s="29"/>
+      <c r="T53" s="29"/>
+      <c r="U53" s="14"/>
+    </row>
+    <row r="54" spans="1:21">
+      <c r="A54" s="10"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="120"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="29"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="29"/>
+      <c r="T54" s="29"/>
+      <c r="U54" s="14"/>
+    </row>
+    <row r="55" spans="1:21">
+      <c r="A55" s="10"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="120"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
+      <c r="Q55" s="30"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="30"/>
+      <c r="T55" s="30"/>
+      <c r="U55" s="14"/>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56" s="10"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="25"/>
+      <c r="M56" s="25"/>
+      <c r="N56" s="120"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="29"/>
+      <c r="R56" s="20"/>
+      <c r="S56" s="29"/>
+      <c r="T56" s="29"/>
+      <c r="U56" s="14"/>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="A57" s="10"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="25"/>
+      <c r="M57" s="25"/>
+      <c r="N57" s="120"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="20"/>
+      <c r="Q57" s="29"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="29"/>
+      <c r="T57" s="29"/>
+      <c r="U57" s="14"/>
+    </row>
+    <row r="58" spans="1:21">
+      <c r="A58" s="10"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="77"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
+      <c r="K58" s="25"/>
+      <c r="L58" s="25"/>
+      <c r="M58" s="25"/>
+      <c r="N58" s="120"/>
+      <c r="O58" s="24"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="29"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="29"/>
+      <c r="T58" s="29"/>
+      <c r="U58" s="14"/>
+    </row>
+    <row r="59" spans="1:21">
+      <c r="A59" s="10"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
+      <c r="K59" s="25"/>
+      <c r="L59" s="25"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="120"/>
+      <c r="O59" s="24"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="29"/>
+      <c r="R59" s="20"/>
+      <c r="S59" s="29"/>
+      <c r="T59" s="29"/>
+      <c r="U59" s="14"/>
+    </row>
+    <row r="60" spans="1:21">
+      <c r="A60" s="10"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="77"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="120"/>
+      <c r="O60" s="24"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="29"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="29"/>
+      <c r="T60" s="29"/>
+      <c r="U60" s="14"/>
+    </row>
+    <row r="61" spans="1:21">
+      <c r="A61" s="10"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="77"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
+      <c r="K61" s="25"/>
+      <c r="L61" s="25"/>
+      <c r="M61" s="25"/>
+      <c r="N61" s="120"/>
+      <c r="O61" s="24"/>
+      <c r="P61" s="24"/>
+      <c r="Q61" s="30"/>
+      <c r="R61" s="24"/>
+      <c r="S61" s="30"/>
+      <c r="T61" s="30"/>
+      <c r="U61" s="14"/>
+    </row>
+    <row r="62" spans="1:21">
+      <c r="A62" s="10"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="77"/>
+      <c r="H62" s="25"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="25"/>
+      <c r="L62" s="25"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="120"/>
+      <c r="O62" s="24"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="29"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="29"/>
+      <c r="T62" s="29"/>
+      <c r="U62" s="14"/>
+    </row>
+    <row r="63" spans="1:21">
+      <c r="A63" s="10"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="77"/>
+      <c r="H63" s="25"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="25"/>
+      <c r="K63" s="25"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="25"/>
+      <c r="N63" s="120"/>
+      <c r="O63" s="24"/>
+      <c r="P63" s="20"/>
+      <c r="Q63" s="29"/>
+      <c r="R63" s="20"/>
+      <c r="S63" s="29"/>
+      <c r="T63" s="29"/>
+      <c r="U63" s="14"/>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64" s="10"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="77"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="120"/>
+      <c r="O64" s="24"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="29"/>
+      <c r="R64" s="20"/>
+      <c r="S64" s="29"/>
+      <c r="T64" s="29"/>
+      <c r="U64" s="14"/>
+    </row>
+    <row r="65" spans="1:21">
+      <c r="A65" s="10"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="77"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="25"/>
+      <c r="L65" s="25"/>
+      <c r="M65" s="25"/>
+      <c r="N65" s="120"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="29"/>
+      <c r="R65" s="20"/>
+      <c r="S65" s="29"/>
+      <c r="T65" s="29"/>
+      <c r="U65" s="14"/>
+    </row>
+    <row r="66" spans="1:21">
+      <c r="A66" s="10"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="77"/>
+      <c r="H66" s="25"/>
+      <c r="I66" s="25"/>
+      <c r="J66" s="25"/>
+      <c r="K66" s="25"/>
+      <c r="L66" s="25"/>
+      <c r="M66" s="25"/>
+      <c r="N66" s="120"/>
+      <c r="O66" s="24"/>
+      <c r="P66" s="24"/>
+      <c r="Q66" s="30"/>
+      <c r="R66" s="24"/>
+      <c r="S66" s="30"/>
+      <c r="T66" s="30"/>
+      <c r="U66" s="14"/>
+    </row>
+    <row r="67" spans="1:21">
+      <c r="A67" s="10"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="25"/>
+      <c r="I67" s="25"/>
+      <c r="J67" s="25"/>
+      <c r="K67" s="25"/>
+      <c r="L67" s="25"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="120"/>
+      <c r="O67" s="24"/>
+      <c r="P67" s="20"/>
+      <c r="Q67" s="29"/>
+      <c r="R67" s="20"/>
+      <c r="S67" s="29"/>
+      <c r="T67" s="29"/>
+      <c r="U67" s="14"/>
+    </row>
+    <row r="68" spans="1:21">
+      <c r="A68" s="10"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="77"/>
+      <c r="H68" s="25"/>
+      <c r="I68" s="25"/>
+      <c r="J68" s="25"/>
+      <c r="K68" s="25"/>
+      <c r="L68" s="25"/>
+      <c r="M68" s="25"/>
+      <c r="N68" s="120"/>
+      <c r="O68" s="24"/>
+      <c r="P68" s="20"/>
+      <c r="Q68" s="29"/>
+      <c r="R68" s="20"/>
+      <c r="S68" s="29"/>
+      <c r="T68" s="29"/>
+      <c r="U68" s="14"/>
+    </row>
+    <row r="69" spans="1:21">
+      <c r="A69" s="10"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="25"/>
+      <c r="I69" s="25"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="25"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="120"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="24"/>
+      <c r="Q69" s="30"/>
+      <c r="R69" s="24"/>
+      <c r="S69" s="30"/>
+      <c r="T69" s="30"/>
+      <c r="U69" s="14"/>
+    </row>
+    <row r="70" spans="1:21">
+      <c r="A70" s="15"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="79"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="26"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="26"/>
+      <c r="M70" s="26"/>
+      <c r="N70" s="120"/>
+      <c r="O70" s="26"/>
+      <c r="P70" s="22"/>
+      <c r="Q70" s="31"/>
+      <c r="R70" s="22"/>
+      <c r="S70" s="31"/>
+      <c r="T70" s="31"/>
+      <c r="U70" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="U45:U46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="O45:O46"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="R45:S45"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
-  <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="portrait"/>
+  <dataValidations count="4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{C5FD77B2-2AE4-264F-8274-7520EEB5F68C}">
+      <formula1>Validate実装パターン</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C23" xr:uid="{C5F2444A-281D-9243-AA29-3185456F643D}">
+      <formula1>isImport</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O47:O70" xr:uid="{30A8D395-EEFA-2742-9F2F-B71285E65A8F}">
+      <formula1>isNullable</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N47:N70" xr:uid="{16CA8BB6-D7FC-CF44-8B37-4D8F010DAA1A}">
+      <formula1>path</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D&amp;  &amp;T</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6BA34B5-61F3-1B45-99E8-F9893D3D6EB3}">
+          <x14:formula1>
+            <xm:f>config!$B$5:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G47:G70</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{5932EB90-7F7A-7541-9CDB-FAC212691337}">
+          <x14:formula1>
+            <xm:f>config!$C$5:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{EF6987E4-FEF4-8441-9D5F-320FDF2BB8A9}">
+          <x14:formula1>
+            <xm:f>config!$D$5:$D$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C10:C12</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0629FD56-9154-5E4F-B15D-CFEB69CD9D77}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="25.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="43.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6.1640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.83203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.83203125" style="1"/>
+    <col min="28" max="28" width="9.1640625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19">
+    <row r="1" spans="1:15" ht="19">
       <c r="A1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="38" t="s">
+    <row r="2" spans="1:15">
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="119" t="str">
+        <f>process!D6&amp;PROPER(C9)&amp;IF(C8="要求電文(C→S)", "Request", "Response")</f>
+        <v>BlancoApiPlainArraySamplePutResponse</v>
+      </c>
+      <c r="D6" s="118"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="G4" s="124" t="s">
-        <v>201</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="39" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="85"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="111"/>
+      <c r="C13" s="151" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="151"/>
+      <c r="E13" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="111" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="111"/>
+      <c r="C14" s="151" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="151"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="113"/>
+      <c r="C15" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="112" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" s="113"/>
+      <c r="C16" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>248</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="146" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="146"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="140" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="141"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="141"/>
+      <c r="F19" s="141"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="101"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="106"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="157"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="107"/>
+      <c r="B21" s="158"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="158"/>
+      <c r="E21" s="158"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="108"/>
+      <c r="B22" s="159"/>
+      <c r="C22" s="159"/>
+      <c r="D22" s="159"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
+      <c r="G22" s="159"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="C23"/>
+      <c r="J23" s="102"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="143" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="144"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="145"/>
+      <c r="J24" s="102"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="164" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="164"/>
+      <c r="D25" s="164"/>
+      <c r="E25" s="164"/>
+      <c r="F25" s="164"/>
+      <c r="G25" s="164"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="P25" s="101"/>
+      <c r="Q25" s="101"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="106">
+        <v>1</v>
+      </c>
+      <c r="B26" s="165" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="165"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="165"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="102"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="107"/>
+      <c r="B27" s="166"/>
+      <c r="C27" s="166"/>
+      <c r="D27" s="166"/>
+      <c r="E27" s="166"/>
+      <c r="F27" s="166"/>
+      <c r="G27" s="166"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="108"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
+      <c r="H28" s="102"/>
+      <c r="I28" s="102"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29" s="102"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="143" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" s="144"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="145"/>
+      <c r="J30" s="102"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="164" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="164"/>
+      <c r="D31" s="164"/>
+      <c r="E31" s="164"/>
+      <c r="F31" s="164"/>
+      <c r="G31" s="164"/>
+      <c r="H31" s="95"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="95"/>
+      <c r="M31" s="95"/>
+      <c r="N31" s="95"/>
+      <c r="P31" s="101"/>
+      <c r="Q31" s="101"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="106"/>
+      <c r="B32" s="157"/>
+      <c r="C32" s="157"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="157"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="168"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
+      <c r="J32"/>
+      <c r="K32" s="102"/>
+      <c r="L32" s="102"/>
+      <c r="M32" s="102"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" s="107"/>
+      <c r="B33" s="158"/>
+      <c r="C33" s="158"/>
+      <c r="D33" s="158"/>
+      <c r="E33" s="158"/>
+      <c r="F33" s="158"/>
+      <c r="G33" s="169"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="K33" s="102"/>
+      <c r="L33" s="102"/>
+      <c r="M33" s="102"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="108"/>
+      <c r="B34" s="159"/>
+      <c r="C34" s="159"/>
+      <c r="D34" s="159"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="159"/>
+      <c r="G34" s="170"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="102"/>
+      <c r="J34" s="95"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35" s="102"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="6"/>
+      <c r="J36" s="102"/>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="116"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="48"/>
+      <c r="P37" s="49"/>
+    </row>
+    <row r="38" spans="1:17" ht="15">
+      <c r="A38" s="181" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="181" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="181" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="181" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="181" t="s">
+        <v>170</v>
+      </c>
+      <c r="G38" s="181" t="s">
+        <v>136</v>
+      </c>
+      <c r="H38" s="181" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="181" t="s">
+        <v>229</v>
+      </c>
+      <c r="J38" s="176" t="s">
+        <v>189</v>
+      </c>
+      <c r="K38" s="186" t="s">
+        <v>119</v>
+      </c>
+      <c r="L38" s="187"/>
+      <c r="M38" s="188" t="s">
+        <v>120</v>
+      </c>
+      <c r="N38" s="187"/>
+      <c r="O38" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="P38" s="181" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15">
+      <c r="A39" s="185"/>
+      <c r="B39" s="185"/>
+      <c r="C39" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="185"/>
+      <c r="E39" s="182"/>
+      <c r="F39" s="182"/>
+      <c r="G39" s="185"/>
+      <c r="H39" s="185"/>
+      <c r="I39" s="185"/>
+      <c r="J39" s="183"/>
+      <c r="K39" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="L39" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="M39" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="N39" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="O39" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="P39" s="185"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="55">
+        <v>1</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="59"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="55">
+        <v>2</v>
+      </c>
+      <c r="B41" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="K41" s="56"/>
+      <c r="L41" s="56"/>
+      <c r="M41" s="56"/>
+      <c r="N41" s="56"/>
+      <c r="O41" s="56"/>
+      <c r="P41" s="59"/>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" s="55">
+        <v>3</v>
+      </c>
+      <c r="B42" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="45"/>
+      <c r="D42" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56"/>
+      <c r="P42" s="62"/>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="55">
+        <v>4</v>
+      </c>
+      <c r="B43" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="64"/>
+      <c r="D43" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="65"/>
+      <c r="J43" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="K43" s="56"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="56"/>
+      <c r="P43" s="66"/>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" s="55">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="125" t="s">
-        <v>202</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="41" t="s">
+      <c r="B44" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="64"/>
+      <c r="D44" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" s="65"/>
+      <c r="G44" s="82"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="66"/>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" s="55">
         <v>6</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="43" t="s">
-        <v>200</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="41" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="126"/>
-      <c r="H7" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="C8" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="D10" s="3"/>
+      <c r="B45" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="64"/>
+      <c r="D45" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="82"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="65"/>
+      <c r="J45" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="66"/>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" s="55">
+        <v>7</v>
+      </c>
+      <c r="B46" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="64"/>
+      <c r="D46" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="66"/>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" s="55"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="65"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="66"/>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" s="55"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="66"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="55"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="65"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="66"/>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="55"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="82"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="65"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="56"/>
+      <c r="P50" s="66"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="55"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="64"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="65"/>
+      <c r="G51" s="82"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="65"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="56"/>
+      <c r="P51" s="66"/>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="55"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="65"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="56"/>
+      <c r="P52" s="66"/>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="55"/>
+      <c r="B53" s="63"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="65"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="56"/>
+      <c r="O53" s="56"/>
+      <c r="P53" s="66"/>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" s="55"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="82"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="65"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
+      <c r="P54" s="66"/>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="55"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="82"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="65"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="56"/>
+      <c r="L55" s="56"/>
+      <c r="M55" s="56"/>
+      <c r="N55" s="56"/>
+      <c r="O55" s="56"/>
+      <c r="P55" s="66"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="55"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="65"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="56"/>
+      <c r="M56" s="56"/>
+      <c r="N56" s="56"/>
+      <c r="O56" s="56"/>
+      <c r="P56" s="66"/>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" s="55"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="65"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="56"/>
+      <c r="M57" s="56"/>
+      <c r="N57" s="56"/>
+      <c r="O57" s="56"/>
+      <c r="P57" s="66"/>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" s="55"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="82"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
+      <c r="O58" s="56"/>
+      <c r="P58" s="66"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="55"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="65"/>
+      <c r="J59" s="24"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
+      <c r="P59" s="66"/>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" s="55"/>
+      <c r="B60" s="63"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="65"/>
+      <c r="F60" s="65"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="65"/>
+      <c r="I60" s="65"/>
+      <c r="J60" s="24"/>
+      <c r="K60" s="56"/>
+      <c r="L60" s="56"/>
+      <c r="M60" s="56"/>
+      <c r="N60" s="56"/>
+      <c r="O60" s="56"/>
+      <c r="P60" s="66"/>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" s="55"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="64"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="82"/>
+      <c r="H61" s="65"/>
+      <c r="I61" s="65"/>
+      <c r="J61" s="24"/>
+      <c r="K61" s="56"/>
+      <c r="L61" s="56"/>
+      <c r="M61" s="56"/>
+      <c r="N61" s="56"/>
+      <c r="O61" s="56"/>
+      <c r="P61" s="66"/>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" s="55"/>
+      <c r="B62" s="63"/>
+      <c r="C62" s="64"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="65"/>
+      <c r="G62" s="82"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="65"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="58"/>
+      <c r="L62" s="58"/>
+      <c r="M62" s="58"/>
+      <c r="N62" s="58"/>
+      <c r="O62" s="58"/>
+      <c r="P62" s="66"/>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" s="67"/>
+      <c r="B63" s="68"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="83"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="71"/>
+      <c r="L63" s="71"/>
+      <c r="M63" s="71"/>
+      <c r="N63" s="71"/>
+      <c r="O63" s="71"/>
+      <c r="P63" s="72"/>
     </row>
   </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="M38:N38"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
+  <dataValidations count="3">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{CDE1C50B-05E1-DD42-B286-7248726D36F1}">
+      <formula1>Validate実装パターン</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16" xr:uid="{CAF88743-2701-5B48-A407-AC5175679ABF}">
+      <formula1>isImport</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J40:J63" xr:uid="{C124E77F-8228-B646-A201-85E8C640C01F}">
+      <formula1>isNullable</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D&amp;  &amp;T</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{872D4F80-8E55-E449-A25F-D0145589C936}">
+          <x14:formula1>
+            <xm:f>config!$B$5:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G40:G63</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{B22FD8D5-DBDA-684C-9A03-0FE4530C1E18}">
+          <x14:formula1>
+            <xm:f>config!$C$5:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>